<commit_message>
Update notes and results
</commit_message>
<xml_diff>
--- a/doc/Div test hit counts.xlsx
+++ b/doc/Div test hit counts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="334"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="334" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Div test hits" sheetId="1" r:id="rId1"/>
@@ -1965,8 +1965,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2033428640"/>
-        <c:axId val="-2033434080"/>
+        <c:axId val="-690721472"/>
+        <c:axId val="-690717120"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -2887,7 +2887,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2033428640"/>
+        <c:axId val="-690721472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2944,12 +2944,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2033434080"/>
+        <c:crossAx val="-690717120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2033434080"/>
+        <c:axId val="-690717120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3006,7 +3006,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2033428640"/>
+        <c:crossAx val="-690721472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3877,8 +3877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11180,7 +11180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S287"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>